<commit_message>
+Methode zur normalisierten Übertragung in DB
</commit_message>
<xml_diff>
--- a/bin/input_output_Excel/INPUT_Testdaten_Personen.xlsx
+++ b/bin/input_output_Excel/INPUT_Testdaten_Personen.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
   <si>
     <t>Vorname0</t>
   </si>
@@ -312,6 +312,906 @@
   </si>
   <si>
     <t>Nachname49</t>
+  </si>
+  <si>
+    <t>Vorname50</t>
+  </si>
+  <si>
+    <t>Nachname50</t>
+  </si>
+  <si>
+    <t>Vorname51</t>
+  </si>
+  <si>
+    <t>Nachname51</t>
+  </si>
+  <si>
+    <t>Vorname52</t>
+  </si>
+  <si>
+    <t>Nachname52</t>
+  </si>
+  <si>
+    <t>Vorname53</t>
+  </si>
+  <si>
+    <t>Nachname53</t>
+  </si>
+  <si>
+    <t>Vorname54</t>
+  </si>
+  <si>
+    <t>Nachname54</t>
+  </si>
+  <si>
+    <t>Vorname55</t>
+  </si>
+  <si>
+    <t>Nachname55</t>
+  </si>
+  <si>
+    <t>Vorname56</t>
+  </si>
+  <si>
+    <t>Nachname56</t>
+  </si>
+  <si>
+    <t>Vorname57</t>
+  </si>
+  <si>
+    <t>Nachname57</t>
+  </si>
+  <si>
+    <t>Vorname58</t>
+  </si>
+  <si>
+    <t>Nachname58</t>
+  </si>
+  <si>
+    <t>Vorname59</t>
+  </si>
+  <si>
+    <t>Nachname59</t>
+  </si>
+  <si>
+    <t>Vorname60</t>
+  </si>
+  <si>
+    <t>Nachname60</t>
+  </si>
+  <si>
+    <t>Vorname61</t>
+  </si>
+  <si>
+    <t>Nachname61</t>
+  </si>
+  <si>
+    <t>Vorname62</t>
+  </si>
+  <si>
+    <t>Nachname62</t>
+  </si>
+  <si>
+    <t>Vorname63</t>
+  </si>
+  <si>
+    <t>Nachname63</t>
+  </si>
+  <si>
+    <t>Vorname64</t>
+  </si>
+  <si>
+    <t>Nachname64</t>
+  </si>
+  <si>
+    <t>Vorname65</t>
+  </si>
+  <si>
+    <t>Nachname65</t>
+  </si>
+  <si>
+    <t>Vorname66</t>
+  </si>
+  <si>
+    <t>Nachname66</t>
+  </si>
+  <si>
+    <t>Vorname67</t>
+  </si>
+  <si>
+    <t>Nachname67</t>
+  </si>
+  <si>
+    <t>Vorname68</t>
+  </si>
+  <si>
+    <t>Nachname68</t>
+  </si>
+  <si>
+    <t>Vorname69</t>
+  </si>
+  <si>
+    <t>Nachname69</t>
+  </si>
+  <si>
+    <t>Vorname70</t>
+  </si>
+  <si>
+    <t>Nachname70</t>
+  </si>
+  <si>
+    <t>Vorname71</t>
+  </si>
+  <si>
+    <t>Nachname71</t>
+  </si>
+  <si>
+    <t>Vorname72</t>
+  </si>
+  <si>
+    <t>Nachname72</t>
+  </si>
+  <si>
+    <t>Vorname73</t>
+  </si>
+  <si>
+    <t>Nachname73</t>
+  </si>
+  <si>
+    <t>Vorname74</t>
+  </si>
+  <si>
+    <t>Nachname74</t>
+  </si>
+  <si>
+    <t>Vorname75</t>
+  </si>
+  <si>
+    <t>Nachname75</t>
+  </si>
+  <si>
+    <t>Vorname76</t>
+  </si>
+  <si>
+    <t>Nachname76</t>
+  </si>
+  <si>
+    <t>Vorname77</t>
+  </si>
+  <si>
+    <t>Nachname77</t>
+  </si>
+  <si>
+    <t>Vorname78</t>
+  </si>
+  <si>
+    <t>Nachname78</t>
+  </si>
+  <si>
+    <t>Vorname79</t>
+  </si>
+  <si>
+    <t>Nachname79</t>
+  </si>
+  <si>
+    <t>Vorname80</t>
+  </si>
+  <si>
+    <t>Nachname80</t>
+  </si>
+  <si>
+    <t>Vorname81</t>
+  </si>
+  <si>
+    <t>Nachname81</t>
+  </si>
+  <si>
+    <t>Vorname82</t>
+  </si>
+  <si>
+    <t>Nachname82</t>
+  </si>
+  <si>
+    <t>Vorname83</t>
+  </si>
+  <si>
+    <t>Nachname83</t>
+  </si>
+  <si>
+    <t>Vorname84</t>
+  </si>
+  <si>
+    <t>Nachname84</t>
+  </si>
+  <si>
+    <t>Vorname85</t>
+  </si>
+  <si>
+    <t>Nachname85</t>
+  </si>
+  <si>
+    <t>Vorname86</t>
+  </si>
+  <si>
+    <t>Nachname86</t>
+  </si>
+  <si>
+    <t>Vorname87</t>
+  </si>
+  <si>
+    <t>Nachname87</t>
+  </si>
+  <si>
+    <t>Vorname88</t>
+  </si>
+  <si>
+    <t>Nachname88</t>
+  </si>
+  <si>
+    <t>Vorname89</t>
+  </si>
+  <si>
+    <t>Nachname89</t>
+  </si>
+  <si>
+    <t>Vorname90</t>
+  </si>
+  <si>
+    <t>Nachname90</t>
+  </si>
+  <si>
+    <t>Vorname91</t>
+  </si>
+  <si>
+    <t>Nachname91</t>
+  </si>
+  <si>
+    <t>Vorname92</t>
+  </si>
+  <si>
+    <t>Nachname92</t>
+  </si>
+  <si>
+    <t>Vorname93</t>
+  </si>
+  <si>
+    <t>Nachname93</t>
+  </si>
+  <si>
+    <t>Vorname94</t>
+  </si>
+  <si>
+    <t>Nachname94</t>
+  </si>
+  <si>
+    <t>Vorname95</t>
+  </si>
+  <si>
+    <t>Nachname95</t>
+  </si>
+  <si>
+    <t>Vorname96</t>
+  </si>
+  <si>
+    <t>Nachname96</t>
+  </si>
+  <si>
+    <t>Vorname97</t>
+  </si>
+  <si>
+    <t>Nachname97</t>
+  </si>
+  <si>
+    <t>Vorname98</t>
+  </si>
+  <si>
+    <t>Nachname98</t>
+  </si>
+  <si>
+    <t>Vorname99</t>
+  </si>
+  <si>
+    <t>Nachname99</t>
+  </si>
+  <si>
+    <t>Vorname100</t>
+  </si>
+  <si>
+    <t>Nachname100</t>
+  </si>
+  <si>
+    <t>Vorname101</t>
+  </si>
+  <si>
+    <t>Nachname101</t>
+  </si>
+  <si>
+    <t>Vorname102</t>
+  </si>
+  <si>
+    <t>Nachname102</t>
+  </si>
+  <si>
+    <t>Vorname103</t>
+  </si>
+  <si>
+    <t>Nachname103</t>
+  </si>
+  <si>
+    <t>Vorname104</t>
+  </si>
+  <si>
+    <t>Nachname104</t>
+  </si>
+  <si>
+    <t>Vorname105</t>
+  </si>
+  <si>
+    <t>Nachname105</t>
+  </si>
+  <si>
+    <t>Vorname106</t>
+  </si>
+  <si>
+    <t>Nachname106</t>
+  </si>
+  <si>
+    <t>Vorname107</t>
+  </si>
+  <si>
+    <t>Nachname107</t>
+  </si>
+  <si>
+    <t>Vorname108</t>
+  </si>
+  <si>
+    <t>Nachname108</t>
+  </si>
+  <si>
+    <t>Vorname109</t>
+  </si>
+  <si>
+    <t>Nachname109</t>
+  </si>
+  <si>
+    <t>Vorname110</t>
+  </si>
+  <si>
+    <t>Nachname110</t>
+  </si>
+  <si>
+    <t>Vorname111</t>
+  </si>
+  <si>
+    <t>Nachname111</t>
+  </si>
+  <si>
+    <t>Vorname112</t>
+  </si>
+  <si>
+    <t>Nachname112</t>
+  </si>
+  <si>
+    <t>Vorname113</t>
+  </si>
+  <si>
+    <t>Nachname113</t>
+  </si>
+  <si>
+    <t>Vorname114</t>
+  </si>
+  <si>
+    <t>Nachname114</t>
+  </si>
+  <si>
+    <t>Vorname115</t>
+  </si>
+  <si>
+    <t>Nachname115</t>
+  </si>
+  <si>
+    <t>Vorname116</t>
+  </si>
+  <si>
+    <t>Nachname116</t>
+  </si>
+  <si>
+    <t>Vorname117</t>
+  </si>
+  <si>
+    <t>Nachname117</t>
+  </si>
+  <si>
+    <t>Vorname118</t>
+  </si>
+  <si>
+    <t>Nachname118</t>
+  </si>
+  <si>
+    <t>Vorname119</t>
+  </si>
+  <si>
+    <t>Nachname119</t>
+  </si>
+  <si>
+    <t>Vorname120</t>
+  </si>
+  <si>
+    <t>Nachname120</t>
+  </si>
+  <si>
+    <t>Vorname121</t>
+  </si>
+  <si>
+    <t>Nachname121</t>
+  </si>
+  <si>
+    <t>Vorname122</t>
+  </si>
+  <si>
+    <t>Nachname122</t>
+  </si>
+  <si>
+    <t>Vorname123</t>
+  </si>
+  <si>
+    <t>Nachname123</t>
+  </si>
+  <si>
+    <t>Vorname124</t>
+  </si>
+  <si>
+    <t>Nachname124</t>
+  </si>
+  <si>
+    <t>Vorname125</t>
+  </si>
+  <si>
+    <t>Nachname125</t>
+  </si>
+  <si>
+    <t>Vorname126</t>
+  </si>
+  <si>
+    <t>Nachname126</t>
+  </si>
+  <si>
+    <t>Vorname127</t>
+  </si>
+  <si>
+    <t>Nachname127</t>
+  </si>
+  <si>
+    <t>Vorname128</t>
+  </si>
+  <si>
+    <t>Nachname128</t>
+  </si>
+  <si>
+    <t>Vorname129</t>
+  </si>
+  <si>
+    <t>Nachname129</t>
+  </si>
+  <si>
+    <t>Vorname130</t>
+  </si>
+  <si>
+    <t>Nachname130</t>
+  </si>
+  <si>
+    <t>Vorname131</t>
+  </si>
+  <si>
+    <t>Nachname131</t>
+  </si>
+  <si>
+    <t>Vorname132</t>
+  </si>
+  <si>
+    <t>Nachname132</t>
+  </si>
+  <si>
+    <t>Vorname133</t>
+  </si>
+  <si>
+    <t>Nachname133</t>
+  </si>
+  <si>
+    <t>Vorname134</t>
+  </si>
+  <si>
+    <t>Nachname134</t>
+  </si>
+  <si>
+    <t>Vorname135</t>
+  </si>
+  <si>
+    <t>Nachname135</t>
+  </si>
+  <si>
+    <t>Vorname136</t>
+  </si>
+  <si>
+    <t>Nachname136</t>
+  </si>
+  <si>
+    <t>Vorname137</t>
+  </si>
+  <si>
+    <t>Nachname137</t>
+  </si>
+  <si>
+    <t>Vorname138</t>
+  </si>
+  <si>
+    <t>Nachname138</t>
+  </si>
+  <si>
+    <t>Vorname139</t>
+  </si>
+  <si>
+    <t>Nachname139</t>
+  </si>
+  <si>
+    <t>Vorname140</t>
+  </si>
+  <si>
+    <t>Nachname140</t>
+  </si>
+  <si>
+    <t>Vorname141</t>
+  </si>
+  <si>
+    <t>Nachname141</t>
+  </si>
+  <si>
+    <t>Vorname142</t>
+  </si>
+  <si>
+    <t>Nachname142</t>
+  </si>
+  <si>
+    <t>Vorname143</t>
+  </si>
+  <si>
+    <t>Nachname143</t>
+  </si>
+  <si>
+    <t>Vorname144</t>
+  </si>
+  <si>
+    <t>Nachname144</t>
+  </si>
+  <si>
+    <t>Vorname145</t>
+  </si>
+  <si>
+    <t>Nachname145</t>
+  </si>
+  <si>
+    <t>Vorname146</t>
+  </si>
+  <si>
+    <t>Nachname146</t>
+  </si>
+  <si>
+    <t>Vorname147</t>
+  </si>
+  <si>
+    <t>Nachname147</t>
+  </si>
+  <si>
+    <t>Vorname148</t>
+  </si>
+  <si>
+    <t>Nachname148</t>
+  </si>
+  <si>
+    <t>Vorname149</t>
+  </si>
+  <si>
+    <t>Nachname149</t>
+  </si>
+  <si>
+    <t>Vorname150</t>
+  </si>
+  <si>
+    <t>Nachname150</t>
+  </si>
+  <si>
+    <t>Vorname151</t>
+  </si>
+  <si>
+    <t>Nachname151</t>
+  </si>
+  <si>
+    <t>Vorname152</t>
+  </si>
+  <si>
+    <t>Nachname152</t>
+  </si>
+  <si>
+    <t>Vorname153</t>
+  </si>
+  <si>
+    <t>Nachname153</t>
+  </si>
+  <si>
+    <t>Vorname154</t>
+  </si>
+  <si>
+    <t>Nachname154</t>
+  </si>
+  <si>
+    <t>Vorname155</t>
+  </si>
+  <si>
+    <t>Nachname155</t>
+  </si>
+  <si>
+    <t>Vorname156</t>
+  </si>
+  <si>
+    <t>Nachname156</t>
+  </si>
+  <si>
+    <t>Vorname157</t>
+  </si>
+  <si>
+    <t>Nachname157</t>
+  </si>
+  <si>
+    <t>Vorname158</t>
+  </si>
+  <si>
+    <t>Nachname158</t>
+  </si>
+  <si>
+    <t>Vorname159</t>
+  </si>
+  <si>
+    <t>Nachname159</t>
+  </si>
+  <si>
+    <t>Vorname160</t>
+  </si>
+  <si>
+    <t>Nachname160</t>
+  </si>
+  <si>
+    <t>Vorname161</t>
+  </si>
+  <si>
+    <t>Nachname161</t>
+  </si>
+  <si>
+    <t>Vorname162</t>
+  </si>
+  <si>
+    <t>Nachname162</t>
+  </si>
+  <si>
+    <t>Vorname163</t>
+  </si>
+  <si>
+    <t>Nachname163</t>
+  </si>
+  <si>
+    <t>Vorname164</t>
+  </si>
+  <si>
+    <t>Nachname164</t>
+  </si>
+  <si>
+    <t>Vorname165</t>
+  </si>
+  <si>
+    <t>Nachname165</t>
+  </si>
+  <si>
+    <t>Vorname166</t>
+  </si>
+  <si>
+    <t>Nachname166</t>
+  </si>
+  <si>
+    <t>Vorname167</t>
+  </si>
+  <si>
+    <t>Nachname167</t>
+  </si>
+  <si>
+    <t>Vorname168</t>
+  </si>
+  <si>
+    <t>Nachname168</t>
+  </si>
+  <si>
+    <t>Vorname169</t>
+  </si>
+  <si>
+    <t>Nachname169</t>
+  </si>
+  <si>
+    <t>Vorname170</t>
+  </si>
+  <si>
+    <t>Nachname170</t>
+  </si>
+  <si>
+    <t>Vorname171</t>
+  </si>
+  <si>
+    <t>Nachname171</t>
+  </si>
+  <si>
+    <t>Vorname172</t>
+  </si>
+  <si>
+    <t>Nachname172</t>
+  </si>
+  <si>
+    <t>Vorname173</t>
+  </si>
+  <si>
+    <t>Nachname173</t>
+  </si>
+  <si>
+    <t>Vorname174</t>
+  </si>
+  <si>
+    <t>Nachname174</t>
+  </si>
+  <si>
+    <t>Vorname175</t>
+  </si>
+  <si>
+    <t>Nachname175</t>
+  </si>
+  <si>
+    <t>Vorname176</t>
+  </si>
+  <si>
+    <t>Nachname176</t>
+  </si>
+  <si>
+    <t>Vorname177</t>
+  </si>
+  <si>
+    <t>Nachname177</t>
+  </si>
+  <si>
+    <t>Vorname178</t>
+  </si>
+  <si>
+    <t>Nachname178</t>
+  </si>
+  <si>
+    <t>Vorname179</t>
+  </si>
+  <si>
+    <t>Nachname179</t>
+  </si>
+  <si>
+    <t>Vorname180</t>
+  </si>
+  <si>
+    <t>Nachname180</t>
+  </si>
+  <si>
+    <t>Vorname181</t>
+  </si>
+  <si>
+    <t>Nachname181</t>
+  </si>
+  <si>
+    <t>Vorname182</t>
+  </si>
+  <si>
+    <t>Nachname182</t>
+  </si>
+  <si>
+    <t>Vorname183</t>
+  </si>
+  <si>
+    <t>Nachname183</t>
+  </si>
+  <si>
+    <t>Vorname184</t>
+  </si>
+  <si>
+    <t>Nachname184</t>
+  </si>
+  <si>
+    <t>Vorname185</t>
+  </si>
+  <si>
+    <t>Nachname185</t>
+  </si>
+  <si>
+    <t>Vorname186</t>
+  </si>
+  <si>
+    <t>Nachname186</t>
+  </si>
+  <si>
+    <t>Vorname187</t>
+  </si>
+  <si>
+    <t>Nachname187</t>
+  </si>
+  <si>
+    <t>Vorname188</t>
+  </si>
+  <si>
+    <t>Nachname188</t>
+  </si>
+  <si>
+    <t>Vorname189</t>
+  </si>
+  <si>
+    <t>Nachname189</t>
+  </si>
+  <si>
+    <t>Vorname190</t>
+  </si>
+  <si>
+    <t>Nachname190</t>
+  </si>
+  <si>
+    <t>Vorname191</t>
+  </si>
+  <si>
+    <t>Nachname191</t>
+  </si>
+  <si>
+    <t>Vorname192</t>
+  </si>
+  <si>
+    <t>Nachname192</t>
+  </si>
+  <si>
+    <t>Vorname193</t>
+  </si>
+  <si>
+    <t>Nachname193</t>
+  </si>
+  <si>
+    <t>Vorname194</t>
+  </si>
+  <si>
+    <t>Nachname194</t>
+  </si>
+  <si>
+    <t>Vorname195</t>
+  </si>
+  <si>
+    <t>Nachname195</t>
+  </si>
+  <si>
+    <t>Vorname196</t>
+  </si>
+  <si>
+    <t>Nachname196</t>
+  </si>
+  <si>
+    <t>Vorname197</t>
+  </si>
+  <si>
+    <t>Nachname197</t>
+  </si>
+  <si>
+    <t>Vorname198</t>
+  </si>
+  <si>
+    <t>Nachname198</t>
+  </si>
+  <si>
+    <t>Vorname199</t>
+  </si>
+  <si>
+    <t>Nachname199</t>
   </si>
 </sst>
 </file>
@@ -356,7 +1256,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -912,6 +1812,1656 @@
         <v>49.0</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" t="s">
+        <v>101</v>
+      </c>
+      <c r="C51" t="n">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" t="n">
+        <v>51.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" t="s">
+        <v>105</v>
+      </c>
+      <c r="C53" t="n">
+        <v>52.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" t="n">
+        <v>53.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" t="n">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" t="s">
+        <v>111</v>
+      </c>
+      <c r="C56" t="n">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" t="n">
+        <v>56.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C58" t="n">
+        <v>57.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" t="n">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" t="s">
+        <v>119</v>
+      </c>
+      <c r="C60" t="n">
+        <v>59.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" t="n">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" t="n">
+        <v>61.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" t="s">
+        <v>125</v>
+      </c>
+      <c r="C63" t="n">
+        <v>62.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" t="n">
+        <v>63.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" t="n">
+        <v>64.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" t="s">
+        <v>131</v>
+      </c>
+      <c r="C66" t="n">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" t="s">
+        <v>133</v>
+      </c>
+      <c r="C67" t="n">
+        <v>66.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" t="n">
+        <v>67.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" t="n">
+        <v>68.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" t="s">
+        <v>139</v>
+      </c>
+      <c r="C70" t="n">
+        <v>69.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
+        <v>141</v>
+      </c>
+      <c r="C71" t="n">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" t="s">
+        <v>143</v>
+      </c>
+      <c r="C72" t="n">
+        <v>71.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" t="s">
+        <v>145</v>
+      </c>
+      <c r="C73" t="n">
+        <v>72.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" t="s">
+        <v>147</v>
+      </c>
+      <c r="C74" t="n">
+        <v>73.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" t="s">
+        <v>149</v>
+      </c>
+      <c r="C75" t="n">
+        <v>74.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" t="s">
+        <v>151</v>
+      </c>
+      <c r="C76" t="n">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
+        <v>153</v>
+      </c>
+      <c r="C77" t="n">
+        <v>76.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>155</v>
+      </c>
+      <c r="C78" t="n">
+        <v>77.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" t="n">
+        <v>78.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" t="s">
+        <v>159</v>
+      </c>
+      <c r="C80" t="n">
+        <v>79.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" t="s">
+        <v>161</v>
+      </c>
+      <c r="C81" t="n">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" t="n">
+        <v>81.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>165</v>
+      </c>
+      <c r="C83" t="n">
+        <v>82.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" t="s">
+        <v>167</v>
+      </c>
+      <c r="C84" t="n">
+        <v>83.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
+        <v>169</v>
+      </c>
+      <c r="C85" t="n">
+        <v>84.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+      <c r="C86" t="n">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" t="s">
+        <v>173</v>
+      </c>
+      <c r="C87" t="n">
+        <v>86.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" t="s">
+        <v>175</v>
+      </c>
+      <c r="C88" t="n">
+        <v>87.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" t="s">
+        <v>177</v>
+      </c>
+      <c r="C89" t="n">
+        <v>88.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" t="s">
+        <v>179</v>
+      </c>
+      <c r="C90" t="n">
+        <v>89.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" t="s">
+        <v>181</v>
+      </c>
+      <c r="C91" t="n">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" t="s">
+        <v>183</v>
+      </c>
+      <c r="C92" t="n">
+        <v>91.0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" t="s">
+        <v>185</v>
+      </c>
+      <c r="C93" t="n">
+        <v>92.0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" t="s">
+        <v>187</v>
+      </c>
+      <c r="C94" t="n">
+        <v>93.0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" t="s">
+        <v>189</v>
+      </c>
+      <c r="C95" t="n">
+        <v>94.0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" t="s">
+        <v>191</v>
+      </c>
+      <c r="C96" t="n">
+        <v>95.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" t="s">
+        <v>193</v>
+      </c>
+      <c r="C97" t="n">
+        <v>96.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" t="s">
+        <v>195</v>
+      </c>
+      <c r="C98" t="n">
+        <v>97.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" t="s">
+        <v>197</v>
+      </c>
+      <c r="C99" t="n">
+        <v>98.0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" t="s">
+        <v>199</v>
+      </c>
+      <c r="C100" t="n">
+        <v>99.0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" t="s">
+        <v>201</v>
+      </c>
+      <c r="C101" t="n">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" t="s">
+        <v>203</v>
+      </c>
+      <c r="C102" t="n">
+        <v>101.0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" t="s">
+        <v>205</v>
+      </c>
+      <c r="C103" t="n">
+        <v>102.0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>206</v>
+      </c>
+      <c r="B104" t="s">
+        <v>207</v>
+      </c>
+      <c r="C104" t="n">
+        <v>103.0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" t="s">
+        <v>209</v>
+      </c>
+      <c r="C105" t="n">
+        <v>104.0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>210</v>
+      </c>
+      <c r="B106" t="s">
+        <v>211</v>
+      </c>
+      <c r="C106" t="n">
+        <v>105.0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>212</v>
+      </c>
+      <c r="B107" t="s">
+        <v>213</v>
+      </c>
+      <c r="C107" t="n">
+        <v>106.0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>214</v>
+      </c>
+      <c r="B108" t="s">
+        <v>215</v>
+      </c>
+      <c r="C108" t="n">
+        <v>107.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>216</v>
+      </c>
+      <c r="B109" t="s">
+        <v>217</v>
+      </c>
+      <c r="C109" t="n">
+        <v>108.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>218</v>
+      </c>
+      <c r="B110" t="s">
+        <v>219</v>
+      </c>
+      <c r="C110" t="n">
+        <v>109.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>220</v>
+      </c>
+      <c r="B111" t="s">
+        <v>221</v>
+      </c>
+      <c r="C111" t="n">
+        <v>110.0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>222</v>
+      </c>
+      <c r="B112" t="s">
+        <v>223</v>
+      </c>
+      <c r="C112" t="n">
+        <v>111.0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>224</v>
+      </c>
+      <c r="B113" t="s">
+        <v>225</v>
+      </c>
+      <c r="C113" t="n">
+        <v>112.0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>226</v>
+      </c>
+      <c r="B114" t="s">
+        <v>227</v>
+      </c>
+      <c r="C114" t="n">
+        <v>113.0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" t="s">
+        <v>229</v>
+      </c>
+      <c r="C115" t="n">
+        <v>114.0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>230</v>
+      </c>
+      <c r="B116" t="s">
+        <v>231</v>
+      </c>
+      <c r="C116" t="n">
+        <v>115.0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>232</v>
+      </c>
+      <c r="B117" t="s">
+        <v>233</v>
+      </c>
+      <c r="C117" t="n">
+        <v>116.0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>234</v>
+      </c>
+      <c r="B118" t="s">
+        <v>235</v>
+      </c>
+      <c r="C118" t="n">
+        <v>117.0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>236</v>
+      </c>
+      <c r="B119" t="s">
+        <v>237</v>
+      </c>
+      <c r="C119" t="n">
+        <v>118.0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>238</v>
+      </c>
+      <c r="B120" t="s">
+        <v>239</v>
+      </c>
+      <c r="C120" t="n">
+        <v>119.0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>240</v>
+      </c>
+      <c r="B121" t="s">
+        <v>241</v>
+      </c>
+      <c r="C121" t="n">
+        <v>120.0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>242</v>
+      </c>
+      <c r="B122" t="s">
+        <v>243</v>
+      </c>
+      <c r="C122" t="n">
+        <v>121.0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" t="s">
+        <v>245</v>
+      </c>
+      <c r="C123" t="n">
+        <v>122.0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>246</v>
+      </c>
+      <c r="B124" t="s">
+        <v>247</v>
+      </c>
+      <c r="C124" t="n">
+        <v>123.0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>248</v>
+      </c>
+      <c r="B125" t="s">
+        <v>249</v>
+      </c>
+      <c r="C125" t="n">
+        <v>124.0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>250</v>
+      </c>
+      <c r="B126" t="s">
+        <v>251</v>
+      </c>
+      <c r="C126" t="n">
+        <v>125.0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>252</v>
+      </c>
+      <c r="B127" t="s">
+        <v>253</v>
+      </c>
+      <c r="C127" t="n">
+        <v>126.0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>254</v>
+      </c>
+      <c r="B128" t="s">
+        <v>255</v>
+      </c>
+      <c r="C128" t="n">
+        <v>127.0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>256</v>
+      </c>
+      <c r="B129" t="s">
+        <v>257</v>
+      </c>
+      <c r="C129" t="n">
+        <v>128.0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>258</v>
+      </c>
+      <c r="B130" t="s">
+        <v>259</v>
+      </c>
+      <c r="C130" t="n">
+        <v>129.0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>260</v>
+      </c>
+      <c r="B131" t="s">
+        <v>261</v>
+      </c>
+      <c r="C131" t="n">
+        <v>130.0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>262</v>
+      </c>
+      <c r="B132" t="s">
+        <v>263</v>
+      </c>
+      <c r="C132" t="n">
+        <v>131.0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>264</v>
+      </c>
+      <c r="B133" t="s">
+        <v>265</v>
+      </c>
+      <c r="C133" t="n">
+        <v>132.0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>266</v>
+      </c>
+      <c r="B134" t="s">
+        <v>267</v>
+      </c>
+      <c r="C134" t="n">
+        <v>133.0</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>268</v>
+      </c>
+      <c r="B135" t="s">
+        <v>269</v>
+      </c>
+      <c r="C135" t="n">
+        <v>134.0</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>270</v>
+      </c>
+      <c r="B136" t="s">
+        <v>271</v>
+      </c>
+      <c r="C136" t="n">
+        <v>135.0</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>272</v>
+      </c>
+      <c r="B137" t="s">
+        <v>273</v>
+      </c>
+      <c r="C137" t="n">
+        <v>136.0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>274</v>
+      </c>
+      <c r="B138" t="s">
+        <v>275</v>
+      </c>
+      <c r="C138" t="n">
+        <v>137.0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>276</v>
+      </c>
+      <c r="B139" t="s">
+        <v>277</v>
+      </c>
+      <c r="C139" t="n">
+        <v>138.0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>278</v>
+      </c>
+      <c r="B140" t="s">
+        <v>279</v>
+      </c>
+      <c r="C140" t="n">
+        <v>139.0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="s">
+        <v>280</v>
+      </c>
+      <c r="B141" t="s">
+        <v>281</v>
+      </c>
+      <c r="C141" t="n">
+        <v>140.0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s">
+        <v>282</v>
+      </c>
+      <c r="B142" t="s">
+        <v>283</v>
+      </c>
+      <c r="C142" t="n">
+        <v>141.0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s">
+        <v>284</v>
+      </c>
+      <c r="B143" t="s">
+        <v>285</v>
+      </c>
+      <c r="C143" t="n">
+        <v>142.0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="s">
+        <v>286</v>
+      </c>
+      <c r="B144" t="s">
+        <v>287</v>
+      </c>
+      <c r="C144" t="n">
+        <v>143.0</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s">
+        <v>288</v>
+      </c>
+      <c r="B145" t="s">
+        <v>289</v>
+      </c>
+      <c r="C145" t="n">
+        <v>144.0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s">
+        <v>290</v>
+      </c>
+      <c r="B146" t="s">
+        <v>291</v>
+      </c>
+      <c r="C146" t="n">
+        <v>145.0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="s">
+        <v>292</v>
+      </c>
+      <c r="B147" t="s">
+        <v>293</v>
+      </c>
+      <c r="C147" t="n">
+        <v>146.0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="s">
+        <v>294</v>
+      </c>
+      <c r="B148" t="s">
+        <v>295</v>
+      </c>
+      <c r="C148" t="n">
+        <v>147.0</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="s">
+        <v>296</v>
+      </c>
+      <c r="B149" t="s">
+        <v>297</v>
+      </c>
+      <c r="C149" t="n">
+        <v>148.0</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="s">
+        <v>298</v>
+      </c>
+      <c r="B150" t="s">
+        <v>299</v>
+      </c>
+      <c r="C150" t="n">
+        <v>149.0</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s">
+        <v>300</v>
+      </c>
+      <c r="B151" t="s">
+        <v>301</v>
+      </c>
+      <c r="C151" t="n">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s">
+        <v>302</v>
+      </c>
+      <c r="B152" t="s">
+        <v>303</v>
+      </c>
+      <c r="C152" t="n">
+        <v>151.0</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s">
+        <v>304</v>
+      </c>
+      <c r="B153" t="s">
+        <v>305</v>
+      </c>
+      <c r="C153" t="n">
+        <v>152.0</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>306</v>
+      </c>
+      <c r="B154" t="s">
+        <v>307</v>
+      </c>
+      <c r="C154" t="n">
+        <v>153.0</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>308</v>
+      </c>
+      <c r="B155" t="s">
+        <v>309</v>
+      </c>
+      <c r="C155" t="n">
+        <v>154.0</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>310</v>
+      </c>
+      <c r="B156" t="s">
+        <v>311</v>
+      </c>
+      <c r="C156" t="n">
+        <v>155.0</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>312</v>
+      </c>
+      <c r="B157" t="s">
+        <v>313</v>
+      </c>
+      <c r="C157" t="n">
+        <v>156.0</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>314</v>
+      </c>
+      <c r="B158" t="s">
+        <v>315</v>
+      </c>
+      <c r="C158" t="n">
+        <v>157.0</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>316</v>
+      </c>
+      <c r="B159" t="s">
+        <v>317</v>
+      </c>
+      <c r="C159" t="n">
+        <v>158.0</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>318</v>
+      </c>
+      <c r="B160" t="s">
+        <v>319</v>
+      </c>
+      <c r="C160" t="n">
+        <v>159.0</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>320</v>
+      </c>
+      <c r="B161" t="s">
+        <v>321</v>
+      </c>
+      <c r="C161" t="n">
+        <v>160.0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>322</v>
+      </c>
+      <c r="B162" t="s">
+        <v>323</v>
+      </c>
+      <c r="C162" t="n">
+        <v>161.0</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>324</v>
+      </c>
+      <c r="B163" t="s">
+        <v>325</v>
+      </c>
+      <c r="C163" t="n">
+        <v>162.0</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>326</v>
+      </c>
+      <c r="B164" t="s">
+        <v>327</v>
+      </c>
+      <c r="C164" t="n">
+        <v>163.0</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>328</v>
+      </c>
+      <c r="B165" t="s">
+        <v>329</v>
+      </c>
+      <c r="C165" t="n">
+        <v>164.0</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>330</v>
+      </c>
+      <c r="B166" t="s">
+        <v>331</v>
+      </c>
+      <c r="C166" t="n">
+        <v>165.0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>332</v>
+      </c>
+      <c r="B167" t="s">
+        <v>333</v>
+      </c>
+      <c r="C167" t="n">
+        <v>166.0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>334</v>
+      </c>
+      <c r="B168" t="s">
+        <v>335</v>
+      </c>
+      <c r="C168" t="n">
+        <v>167.0</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>336</v>
+      </c>
+      <c r="B169" t="s">
+        <v>337</v>
+      </c>
+      <c r="C169" t="n">
+        <v>168.0</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>338</v>
+      </c>
+      <c r="B170" t="s">
+        <v>339</v>
+      </c>
+      <c r="C170" t="n">
+        <v>169.0</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>340</v>
+      </c>
+      <c r="B171" t="s">
+        <v>341</v>
+      </c>
+      <c r="C171" t="n">
+        <v>170.0</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>342</v>
+      </c>
+      <c r="B172" t="s">
+        <v>343</v>
+      </c>
+      <c r="C172" t="n">
+        <v>171.0</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>344</v>
+      </c>
+      <c r="B173" t="s">
+        <v>345</v>
+      </c>
+      <c r="C173" t="n">
+        <v>172.0</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>346</v>
+      </c>
+      <c r="B174" t="s">
+        <v>347</v>
+      </c>
+      <c r="C174" t="n">
+        <v>173.0</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>348</v>
+      </c>
+      <c r="B175" t="s">
+        <v>349</v>
+      </c>
+      <c r="C175" t="n">
+        <v>174.0</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>350</v>
+      </c>
+      <c r="B176" t="s">
+        <v>351</v>
+      </c>
+      <c r="C176" t="n">
+        <v>175.0</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="s">
+        <v>352</v>
+      </c>
+      <c r="B177" t="s">
+        <v>353</v>
+      </c>
+      <c r="C177" t="n">
+        <v>176.0</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="s">
+        <v>354</v>
+      </c>
+      <c r="B178" t="s">
+        <v>355</v>
+      </c>
+      <c r="C178" t="n">
+        <v>177.0</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="s">
+        <v>356</v>
+      </c>
+      <c r="B179" t="s">
+        <v>357</v>
+      </c>
+      <c r="C179" t="n">
+        <v>178.0</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="s">
+        <v>358</v>
+      </c>
+      <c r="B180" t="s">
+        <v>359</v>
+      </c>
+      <c r="C180" t="n">
+        <v>179.0</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="s">
+        <v>360</v>
+      </c>
+      <c r="B181" t="s">
+        <v>361</v>
+      </c>
+      <c r="C181" t="n">
+        <v>180.0</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="s">
+        <v>362</v>
+      </c>
+      <c r="B182" t="s">
+        <v>363</v>
+      </c>
+      <c r="C182" t="n">
+        <v>181.0</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="s">
+        <v>364</v>
+      </c>
+      <c r="B183" t="s">
+        <v>365</v>
+      </c>
+      <c r="C183" t="n">
+        <v>182.0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="s">
+        <v>366</v>
+      </c>
+      <c r="B184" t="s">
+        <v>367</v>
+      </c>
+      <c r="C184" t="n">
+        <v>183.0</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="s">
+        <v>368</v>
+      </c>
+      <c r="B185" t="s">
+        <v>369</v>
+      </c>
+      <c r="C185" t="n">
+        <v>184.0</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="s">
+        <v>370</v>
+      </c>
+      <c r="B186" t="s">
+        <v>371</v>
+      </c>
+      <c r="C186" t="n">
+        <v>185.0</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="s">
+        <v>372</v>
+      </c>
+      <c r="B187" t="s">
+        <v>373</v>
+      </c>
+      <c r="C187" t="n">
+        <v>186.0</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="s">
+        <v>374</v>
+      </c>
+      <c r="B188" t="s">
+        <v>375</v>
+      </c>
+      <c r="C188" t="n">
+        <v>187.0</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="s">
+        <v>376</v>
+      </c>
+      <c r="B189" t="s">
+        <v>377</v>
+      </c>
+      <c r="C189" t="n">
+        <v>188.0</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="s">
+        <v>378</v>
+      </c>
+      <c r="B190" t="s">
+        <v>379</v>
+      </c>
+      <c r="C190" t="n">
+        <v>189.0</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="s">
+        <v>380</v>
+      </c>
+      <c r="B191" t="s">
+        <v>381</v>
+      </c>
+      <c r="C191" t="n">
+        <v>190.0</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="s">
+        <v>382</v>
+      </c>
+      <c r="B192" t="s">
+        <v>383</v>
+      </c>
+      <c r="C192" t="n">
+        <v>191.0</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="s">
+        <v>384</v>
+      </c>
+      <c r="B193" t="s">
+        <v>385</v>
+      </c>
+      <c r="C193" t="n">
+        <v>192.0</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="s">
+        <v>386</v>
+      </c>
+      <c r="B194" t="s">
+        <v>387</v>
+      </c>
+      <c r="C194" t="n">
+        <v>193.0</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="s">
+        <v>388</v>
+      </c>
+      <c r="B195" t="s">
+        <v>389</v>
+      </c>
+      <c r="C195" t="n">
+        <v>194.0</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="s">
+        <v>390</v>
+      </c>
+      <c r="B196" t="s">
+        <v>391</v>
+      </c>
+      <c r="C196" t="n">
+        <v>195.0</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="s">
+        <v>392</v>
+      </c>
+      <c r="B197" t="s">
+        <v>393</v>
+      </c>
+      <c r="C197" t="n">
+        <v>196.0</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="s">
+        <v>394</v>
+      </c>
+      <c r="B198" t="s">
+        <v>395</v>
+      </c>
+      <c r="C198" t="n">
+        <v>197.0</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="s">
+        <v>396</v>
+      </c>
+      <c r="B199" t="s">
+        <v>397</v>
+      </c>
+      <c r="C199" t="n">
+        <v>198.0</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="s">
+        <v>398</v>
+      </c>
+      <c r="B200" t="s">
+        <v>399</v>
+      </c>
+      <c r="C200" t="n">
+        <v>199.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>